<commit_message>
Uppdatering av vision osv
</commit_message>
<xml_diff>
--- a/Krav.xlsx
+++ b/Krav.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
   <si>
     <t>Krav</t>
   </si>
@@ -54,18 +54,12 @@
     <t>AF1.4 Ta bort ett videoklipp</t>
   </si>
   <si>
-    <t>BK1</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
     <t>Användare</t>
   </si>
   <si>
-    <t>B2 Databas</t>
-  </si>
-  <si>
     <t>F1 Inloggning via Facebook</t>
   </si>
   <si>
@@ -75,29 +69,35 @@
     <t>AF1.5 Kommentar via Facebook</t>
   </si>
   <si>
-    <t>AF1.6 Betygsättning</t>
-  </si>
-  <si>
     <t>AF 1.7 Kategorier</t>
   </si>
   <si>
     <t>AF1.8 Redigera ett videoklipp</t>
   </si>
   <si>
-    <t>Not done</t>
-  </si>
-  <si>
-    <t>BK2, BK1</t>
-  </si>
-  <si>
     <t>AF1.9 Redigera bild</t>
+  </si>
+  <si>
+    <t>BK1, BK5</t>
+  </si>
+  <si>
+    <t>BK1, BK2</t>
+  </si>
+  <si>
+    <t>BK1, BK3</t>
+  </si>
+  <si>
+    <t>BK1, BK2, BK3</t>
+  </si>
+  <si>
+    <t>B1 Databas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,6 +226,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -260,6 +261,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -435,14 +437,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
@@ -453,7 +455,7 @@
     <col min="7" max="7" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,248 +479,225 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G2">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G5">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
         <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
       </c>
       <c r="G8">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G10">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
         <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
       </c>
       <c r="G11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G12">
         <v>5</v>
@@ -731,24 +710,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>